<commit_message>
incorporated gbm2_1 model into the stack
</commit_message>
<xml_diff>
--- a/model_results/ConsolidatedModelPerformance.xlsx
+++ b/model_results/ConsolidatedModelPerformance.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="520" windowWidth="25040" windowHeight="15860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ConsolidatedModelPerformance.ts" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="243">
   <si>
     <t>dir</t>
   </si>
@@ -588,6 +588,48 @@
     <t>Class_1.n.trees=150,Class_1.interaction.depth=4,Class_1.shrinkage=0.1,Class_2.n.trees=150,Class_2.interaction.depth=4,Class_2.shrinkage=0.1,Class_3.n.trees=250,Class_3.interaction.depth=3,Class_3.shrinkage=0.1,Class_4.n.trees=200,Class_4.interaction.depth=2,Class_4.shrinkage=0.1,Class_5.n.trees=100,Class_5.interaction.depth=1,Class_5.shrinkage=0.1,Class_6.n.trees=250,Class_6.interaction.depth=3,Class_6.shrinkage=0.1,Class_7.n.trees=250,Class_7.interaction.depth=5,Class_7.shrinkage=0.1,Class_8.n.trees=250,Class_8.interaction.depth=5,Class_8.shrinkage=0.1,Class_9.n.trees=200,Class_9.interaction.depth=5,Class_9.shrinkage=0.1</t>
   </si>
   <si>
+    <t>Class_1.n.trees=100,Class_1.interaction.depth=4,Class_1.shrinkage=0.1,Class_2.n.trees=100,Class_2.interaction.depth=4,Class_2.shrinkage=0.1,Class_3.n.trees=100,Class_3.interaction.depth=5,Class_3.shrinkage=0.1,Class_4.n.trees=50,Class_4.interaction.depth=4,Class_4.shrinkage=0.1,Class_5.n.trees=250,Class_5.interaction.depth=1,Class_5.shrinkage=0.1,Class_6.n.trees=50,Class_6.interaction.depth=4,Class_6.shrinkage=0.1,Class_7.n.trees=150,Class_7.interaction.depth=5,Class_7.shrinkage=0.1,Class_8.n.trees=250,Class_8.interaction.depth=3,Class_8.shrinkage=0.1,Class_9.n.trees=250,Class_9.interaction.depth=4,Class_9.shrinkage=0.1</t>
+  </si>
+  <si>
+    <t>rf1_1.Class_1,rf1_1.Class_2,rf1_1.Class_3,rf1_1.Class_4,rf1_1.Class_5,rf1_1.Class_6,rf1_1.Class_7,rf1_1.Class_8,rf1_1.Class_9,gbm1_1.Class_1,gbm1_1.Class_2,gbm1_1.Class_3,gbm1_1.Class_4,gbm1_1.Class_5,gbm1_1.Class_6,gbm1_1.Class_7,gbm1_1.Class_8,gbm1_1.Class_9,gbm2_1.gbm1_1.Class_1,gbm2_1.gbm1_1.Class_2,gbm2_1.gbm1_1.Class_3,gbm2_1.gbm1_1.Class_4,gbm2_1.gbm1_1.Class_5,gbm2_1.gbm1_1.Class_6,gbm2_1.gbm1_1.Class_7,gbm2_1.gbm1_1.Class_8,gbm2_1.gbm1_1.Class_9,feat_1,feat_2,feat_3,feat_4,feat_5,feat_6,feat_7,feat_8,feat_9,feat_10,feat_11,feat_12,feat_13,feat_14,feat_15,feat_16,feat_17,feat_18,feat_19,feat_20,feat_21,feat_22,feat_23,feat_24,feat_25,feat_26,feat_27,feat_28,feat_29,feat_30,feat_31,feat_32,feat_33,feat_34,feat_35,feat_36,feat_37,feat_38,feat_39,feat_40,feat_41,feat_42,feat_43,feat_44,feat_45,feat_46,feat_47,feat_48,feat_49,feat_50,feat_51,feat_52,feat_53,feat_54,feat_55,feat_56,feat_57,feat_58,feat_59,feat_60,feat_61,feat_62,feat_63,feat_64,feat_65,feat_66,feat_67,feat_68,feat_69,feat_70,feat_71,feat_72,feat_73,feat_74,feat_75,feat_76,feat_77,feat_78,feat_79,feat_80,feat_81,feat_82,feat_83,feat_84,feat_85,feat_86,feat_87,feat_88,feat_89,feat_90,feat_91,feat_92,feat_93,non.zero.count</t>
+  </si>
+  <si>
+    <t>./src/stk_model/gbm2_1</t>
+  </si>
+  <si>
+    <t>Class_1.n.trees=250,Class_1.interaction.depth=5,Class_1.shrinkage=0.1,Class_2.n.trees=250,Class_2.interaction.depth=5,Class_2.shrinkage=0.1,Class_3.n.trees=250,Class_3.interaction.depth=5,Class_3.shrinkage=0.1,Class_4.n.trees=250,Class_4.interaction.depth=5,Class_4.shrinkage=0.1,Class_5.n.trees=250,Class_5.interaction.depth=2,Class_5.shrinkage=0.1,Class_6.n.trees=250,Class_6.interaction.depth=5,Class_6.shrinkage=0.1,Class_7.n.trees=250,Class_7.interaction.depth=4,Class_7.shrinkage=0.1,Class_8.n.trees=250,Class_8.interaction.depth=5,Class_8.shrinkage=0.1,Class_9.n.trees=250,Class_9.interaction.depth=5,Class_9.shrinkage=0.1</t>
+  </si>
+  <si>
+    <t>gbm one vs all default n.minobsinode=10</t>
+  </si>
+  <si>
+    <t>Class_1.n.trees=250,Class_1.interaction.depth=4,Class_1.shrinkage=0.1,Class_2.n.trees=250,Class_2.interaction.depth=5,Class_2.shrinkage=0.1,Class_3.n.trees=250,Class_3.interaction.depth=5,Class_3.shrinkage=0.1,Class_4.n.trees=250,Class_4.interaction.depth=5,Class_4.shrinkage=0.1,Class_5.n.trees=250,Class_5.interaction.depth=1,Class_5.shrinkage=0.1,Class_6.n.trees=250,Class_6.interaction.depth=5,Class_6.shrinkage=0.1,Class_7.n.trees=250,Class_7.interaction.depth=4,Class_7.shrinkage=0.1,Class_8.n.trees=250,Class_8.interaction.depth=5,Class_8.shrinkage=0.1,Class_9.n.trees=250,Class_9.interaction.depth=5,Class_9.shrinkage=0.1</t>
+  </si>
+  <si>
+    <t>verbose=FALSE,n.minobsinnode=5</t>
+  </si>
+  <si>
+    <t>gbm one vs all default n.minobsinnode=5</t>
+  </si>
+  <si>
+    <t>Class_1.n.trees=250,Class_1.interaction.depth=4,Class_1.shrinkage=0.1,Class_2.n.trees=250,Class_2.interaction.depth=5,Class_2.shrinkage=0.1,Class_3.n.trees=250,Class_3.interaction.depth=5,Class_3.shrinkage=0.1,Class_4.n.trees=250,Class_4.interaction.depth=5,Class_4.shrinkage=0.1,Class_5.n.trees=200,Class_5.interaction.depth=5,Class_5.shrinkage=0.1,Class_6.n.trees=250,Class_6.interaction.depth=5,Class_6.shrinkage=0.1,Class_7.n.trees=250,Class_7.interaction.depth=5,Class_7.shrinkage=0.1,Class_8.n.trees=250,Class_8.interaction.depth=5,Class_8.shrinkage=0.1,Class_9.n.trees=250,Class_9.interaction.depth=5,Class_9.shrinkage=0.1</t>
+  </si>
+  <si>
+    <t>verbose=FALSE,n.minobsinnode=15</t>
+  </si>
+  <si>
+    <t>gbm one vs all default n.minobsinnode=15</t>
+  </si>
+  <si>
+    <t>Class_1.n.trees=250,Class_1.interaction.depth=4,Class_1.shrinkage=0.1,Class_2.n.trees=250,Class_2.interaction.depth=5,Class_2.shrinkage=0.1,Class_3.n.trees=250,Class_3.interaction.depth=5,Class_3.shrinkage=0.1,Class_4.n.trees=250,Class_4.interaction.depth=5,Class_4.shrinkage=0.1,Class_5.n.trees=250,Class_5.interaction.depth=4,Class_5.shrinkage=0.1,Class_6.n.trees=250,Class_6.interaction.depth=5,Class_6.shrinkage=0.1,Class_7.n.trees=250,Class_7.interaction.depth=5,Class_7.shrinkage=0.1,Class_8.n.trees=250,Class_8.interaction.depth=5,Class_8.shrinkage=0.1,Class_9.n.trees=250,Class_9.interaction.depth=4,Class_9.shrinkage=0.1</t>
+  </si>
+  <si>
+    <t>verbose=FALSE,n.minobsinnode=20</t>
+  </si>
+  <si>
+    <t>gbm one vs all default n.minobsinnode=20</t>
+  </si>
+  <si>
     <t>./src/stk_model/rf1_1</t>
   </si>
   <si>
@@ -598,6 +640,9 @@
   </si>
   <si>
     <t>Level 2 rf model for model stacking</t>
+  </si>
+  <si>
+    <t>mtry=61</t>
   </si>
   <si>
     <t>./src/svm_model</t>
@@ -758,8 +803,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O184" totalsRowShown="0">
-  <autoFilter ref="A1:O184"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O191" totalsRowShown="0">
+  <autoFilter ref="A1:O191"/>
   <tableColumns count="15">
     <tableColumn id="1" name="dir"/>
     <tableColumn id="2" name="date.time" dataDxfId="0"/>
@@ -1103,15 +1148,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O184"/>
+  <dimension ref="A1:O191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
@@ -1176,7 +1221,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="1">
-        <v>40662.262199074074</v>
+        <v>42124.262199074074</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -1217,7 +1262,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="1">
-        <v>40662.279085648152</v>
+        <v>42124.279085648152</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -1258,7 +1303,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="1">
-        <v>40662.303981481484</v>
+        <v>42124.303981481484</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -1299,7 +1344,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>40662.897407407407</v>
+        <v>42124.897407407407</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -1340,7 +1385,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="1">
-        <v>40662.904675925929</v>
+        <v>42124.904675925929</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -1381,7 +1426,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="1">
-        <v>40662.928738425922</v>
+        <v>42124.928738425922</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -1422,7 +1467,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>40663.886111111111</v>
+        <v>42125.886111111111</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -1463,7 +1508,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="1">
-        <v>40663.894259259258</v>
+        <v>42125.894259259258</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -1504,7 +1549,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="1">
-        <v>40663.907569444447</v>
+        <v>42125.907569444447</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -1545,7 +1590,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="1">
-        <v>40663.913171296299</v>
+        <v>42125.913171296299</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -1586,7 +1631,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="1">
-        <v>40664.134918981479</v>
+        <v>42126.134918981479</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -1627,7 +1672,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>40664.531724537039</v>
+        <v>42126.531724537039</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -1668,7 +1713,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="1">
-        <v>40639.758009259262</v>
+        <v>42101.758009259262</v>
       </c>
       <c r="C14" t="s">
         <v>30</v>
@@ -1703,7 +1748,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="1">
-        <v>40639.762152777781</v>
+        <v>42101.762152777781</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -1738,7 +1783,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="1">
-        <v>40639.763333333336</v>
+        <v>42101.763333333336</v>
       </c>
       <c r="C16" t="s">
         <v>30</v>
@@ -1773,7 +1818,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="1">
-        <v>40639.883819444447</v>
+        <v>42101.883819444447</v>
       </c>
       <c r="C17" t="s">
         <v>30</v>
@@ -1808,7 +1853,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="1">
-        <v>40639.932210648149</v>
+        <v>42101.932210648149</v>
       </c>
       <c r="C18" t="s">
         <v>30</v>
@@ -1843,7 +1888,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="1">
-        <v>40640.874699074076</v>
+        <v>42102.874699074076</v>
       </c>
       <c r="C19" t="s">
         <v>30</v>
@@ -1878,7 +1923,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="1">
-        <v>40647.942337962966</v>
+        <v>42109.942337962966</v>
       </c>
       <c r="C20" t="s">
         <v>30</v>
@@ -1919,7 +1964,7 @@
         <v>29</v>
       </c>
       <c r="B21" s="1">
-        <v>40647.944432870368</v>
+        <v>42109.944432870368</v>
       </c>
       <c r="C21" t="s">
         <v>30</v>
@@ -1960,7 +2005,7 @@
         <v>29</v>
       </c>
       <c r="B22" s="1">
-        <v>40647.945636574077</v>
+        <v>42109.945636574077</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
@@ -2004,7 +2049,7 @@
         <v>29</v>
       </c>
       <c r="B23" s="1">
-        <v>40649.846215277779</v>
+        <v>42111.846215277779</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
@@ -2048,7 +2093,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="1">
-        <v>40649.85328703704</v>
+        <v>42111.85328703704</v>
       </c>
       <c r="C24" t="s">
         <v>30</v>
@@ -2095,7 +2140,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="1">
-        <v>40649.876226851855</v>
+        <v>42111.876226851855</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
@@ -2142,7 +2187,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="1">
-        <v>40652.750289351854</v>
+        <v>42114.750289351854</v>
       </c>
       <c r="C26" t="s">
         <v>30</v>
@@ -2186,7 +2231,7 @@
         <v>29</v>
       </c>
       <c r="B27" s="1">
-        <v>40652.759942129633</v>
+        <v>42114.759942129633</v>
       </c>
       <c r="C27" t="s">
         <v>30</v>
@@ -2233,7 +2278,7 @@
         <v>29</v>
       </c>
       <c r="B28" s="1">
-        <v>40652.7653587963</v>
+        <v>42114.7653587963</v>
       </c>
       <c r="C28" t="s">
         <v>30</v>
@@ -2280,7 +2325,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="1">
-        <v>40652.835798611108</v>
+        <v>42114.835798611108</v>
       </c>
       <c r="C29" t="s">
         <v>30</v>
@@ -2327,7 +2372,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>40652.839166666665</v>
+        <v>42114.839166666665</v>
       </c>
       <c r="C30" t="s">
         <v>30</v>
@@ -2374,7 +2419,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1">
-        <v>40652.848761574074</v>
+        <v>42114.848761574074</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>
@@ -2421,7 +2466,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="1">
-        <v>40661.148125</v>
+        <v>42123.148125</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
@@ -2462,7 +2507,7 @@
         <v>55</v>
       </c>
       <c r="B33" s="1">
-        <v>40646.850069444445</v>
+        <v>42108.850069444445</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
@@ -2497,7 +2542,7 @@
         <v>55</v>
       </c>
       <c r="B34" s="1">
-        <v>40646.875208333331</v>
+        <v>42108.875208333331</v>
       </c>
       <c r="C34" t="s">
         <v>30</v>
@@ -2532,7 +2577,7 @@
         <v>55</v>
       </c>
       <c r="B35" s="1">
-        <v>40646.899583333332</v>
+        <v>42108.899583333332</v>
       </c>
       <c r="C35" t="s">
         <v>30</v>
@@ -2567,7 +2612,7 @@
         <v>55</v>
       </c>
       <c r="B36" s="1">
-        <v>40646.939062500001</v>
+        <v>42108.939062500001</v>
       </c>
       <c r="C36" t="s">
         <v>30</v>
@@ -2602,7 +2647,7 @@
         <v>55</v>
       </c>
       <c r="B37" s="1">
-        <v>40648.013703703706</v>
+        <v>42110.013703703706</v>
       </c>
       <c r="C37" t="s">
         <v>30</v>
@@ -2649,7 +2694,7 @@
         <v>55</v>
       </c>
       <c r="B38" s="1">
-        <v>40648.014513888891</v>
+        <v>42110.014513888891</v>
       </c>
       <c r="C38" t="s">
         <v>30</v>
@@ -2696,7 +2741,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="1">
-        <v>40651.539988425924</v>
+        <v>42113.539988425924</v>
       </c>
       <c r="C39" t="s">
         <v>30</v>
@@ -2743,7 +2788,7 @@
         <v>55</v>
       </c>
       <c r="B40" s="1">
-        <v>40652.868472222224</v>
+        <v>42114.868472222224</v>
       </c>
       <c r="C40" t="s">
         <v>30</v>
@@ -2790,7 +2835,7 @@
         <v>55</v>
       </c>
       <c r="B41" s="1">
-        <v>40652.928113425929</v>
+        <v>42114.928113425929</v>
       </c>
       <c r="C41" t="s">
         <v>30</v>
@@ -2837,7 +2882,7 @@
         <v>55</v>
       </c>
       <c r="B42" s="1">
-        <v>40652.988958333335</v>
+        <v>42114.988958333335</v>
       </c>
       <c r="C42" t="s">
         <v>30</v>
@@ -2884,7 +2929,7 @@
         <v>55</v>
       </c>
       <c r="B43" s="1">
-        <v>40654.282939814817</v>
+        <v>42116.282939814817</v>
       </c>
       <c r="C43" t="s">
         <v>30</v>
@@ -2931,7 +2976,7 @@
         <v>55</v>
       </c>
       <c r="B44" s="1">
-        <v>40654.294745370367</v>
+        <v>42116.294745370367</v>
       </c>
       <c r="C44" t="s">
         <v>30</v>
@@ -2978,7 +3023,7 @@
         <v>55</v>
       </c>
       <c r="B45" s="1">
-        <v>40654.319178240738</v>
+        <v>42116.319178240738</v>
       </c>
       <c r="C45" t="s">
         <v>30</v>
@@ -3025,7 +3070,7 @@
         <v>55</v>
       </c>
       <c r="B46" s="1">
-        <v>40664.956990740742</v>
+        <v>42126.956990740742</v>
       </c>
       <c r="C46" t="s">
         <v>30</v>
@@ -3069,7 +3114,7 @@
         <v>55</v>
       </c>
       <c r="B47" s="1">
-        <v>40664.964074074072</v>
+        <v>42126.964074074072</v>
       </c>
       <c r="C47" t="s">
         <v>30</v>
@@ -3113,7 +3158,7 @@
         <v>55</v>
       </c>
       <c r="B48" s="1">
-        <v>40664.973819444444</v>
+        <v>42126.973819444444</v>
       </c>
       <c r="C48" t="s">
         <v>30</v>
@@ -3157,7 +3202,7 @@
         <v>55</v>
       </c>
       <c r="B49" s="1">
-        <v>40665.273530092592</v>
+        <v>42127.273530092592</v>
       </c>
       <c r="C49" t="s">
         <v>30</v>
@@ -3201,7 +3246,7 @@
         <v>55</v>
       </c>
       <c r="B50" s="1">
-        <v>40665.792708333334</v>
+        <v>42127.792708333334</v>
       </c>
       <c r="C50" t="s">
         <v>30</v>
@@ -3245,7 +3290,7 @@
         <v>55</v>
       </c>
       <c r="B51" s="1">
-        <v>40665.892245370371</v>
+        <v>42127.892245370371</v>
       </c>
       <c r="C51" t="s">
         <v>30</v>
@@ -3289,7 +3334,7 @@
         <v>55</v>
       </c>
       <c r="B52" s="1">
-        <v>40667.467453703706</v>
+        <v>42129.467453703706</v>
       </c>
       <c r="C52" t="s">
         <v>30</v>
@@ -3333,7 +3378,7 @@
         <v>55</v>
       </c>
       <c r="B53" s="1">
-        <v>40668.054444444446</v>
+        <v>42130.054444444446</v>
       </c>
       <c r="C53" t="s">
         <v>30</v>
@@ -3377,7 +3422,7 @@
         <v>55</v>
       </c>
       <c r="B54" s="1">
-        <v>40668.983032407406</v>
+        <v>42130.983032407406</v>
       </c>
       <c r="C54" t="s">
         <v>30</v>
@@ -3421,7 +3466,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="1">
-        <v>40669.452013888891</v>
+        <v>42131.452013888891</v>
       </c>
       <c r="C55" t="s">
         <v>30</v>
@@ -3465,7 +3510,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1">
-        <v>40669.909004629626</v>
+        <v>42131.909004629626</v>
       </c>
       <c r="C56" t="s">
         <v>30</v>
@@ -3509,7 +3554,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="1">
-        <v>40670.011689814812</v>
+        <v>42132.011689814812</v>
       </c>
       <c r="C57" t="s">
         <v>30</v>
@@ -3553,7 +3598,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="1">
-        <v>40670.112511574072</v>
+        <v>42132.112511574072</v>
       </c>
       <c r="C58" t="s">
         <v>30</v>
@@ -3597,7 +3642,7 @@
         <v>55</v>
       </c>
       <c r="B59" s="1">
-        <v>40670.958136574074</v>
+        <v>42132.958136574074</v>
       </c>
       <c r="C59" t="s">
         <v>30</v>
@@ -3641,7 +3686,7 @@
         <v>55</v>
       </c>
       <c r="B60" s="1">
-        <v>40671.95034722222</v>
+        <v>42133.95034722222</v>
       </c>
       <c r="C60" t="s">
         <v>30</v>
@@ -3685,7 +3730,7 @@
         <v>55</v>
       </c>
       <c r="B61" s="1">
-        <v>40671.958773148152</v>
+        <v>42133.958773148152</v>
       </c>
       <c r="C61" t="s">
         <v>30</v>
@@ -3729,7 +3774,7 @@
         <v>55</v>
       </c>
       <c r="B62" s="1">
-        <v>40671.960601851853</v>
+        <v>42133.960601851853</v>
       </c>
       <c r="C62" t="s">
         <v>30</v>
@@ -3773,7 +3818,7 @@
         <v>94</v>
       </c>
       <c r="B63" s="1">
-        <v>40650.427997685183</v>
+        <v>42112.427997685183</v>
       </c>
       <c r="C63" t="s">
         <v>30</v>
@@ -3814,7 +3859,7 @@
         <v>97</v>
       </c>
       <c r="B64" s="1">
-        <v>40673.853414351855</v>
+        <v>42135.853414351855</v>
       </c>
       <c r="C64" t="s">
         <v>30</v>
@@ -3858,7 +3903,7 @@
         <v>97</v>
       </c>
       <c r="B65" s="1">
-        <v>40673.873495370368</v>
+        <v>42135.873495370368</v>
       </c>
       <c r="C65" t="s">
         <v>30</v>
@@ -3902,7 +3947,7 @@
         <v>97</v>
       </c>
       <c r="B66" s="1">
-        <v>40673.918078703704</v>
+        <v>42135.918078703704</v>
       </c>
       <c r="C66" t="s">
         <v>30</v>
@@ -3946,7 +3991,7 @@
         <v>97</v>
       </c>
       <c r="B67" s="1">
-        <v>40674.129525462966</v>
+        <v>42136.129525462966</v>
       </c>
       <c r="C67" t="s">
         <v>30</v>
@@ -3990,7 +4035,7 @@
         <v>97</v>
       </c>
       <c r="B68" s="1">
-        <v>40674.248287037037</v>
+        <v>42136.248287037037</v>
       </c>
       <c r="C68" t="s">
         <v>30</v>
@@ -4034,7 +4079,7 @@
         <v>97</v>
       </c>
       <c r="B69" s="1">
-        <v>40674.686736111114</v>
+        <v>42136.686736111114</v>
       </c>
       <c r="C69" t="s">
         <v>30</v>
@@ -4078,7 +4123,7 @@
         <v>97</v>
       </c>
       <c r="B70" s="1">
-        <v>40675.033009259256</v>
+        <v>42137.033009259256</v>
       </c>
       <c r="C70" t="s">
         <v>30</v>
@@ -4122,7 +4167,7 @@
         <v>97</v>
       </c>
       <c r="B71" s="1">
-        <v>40675.392337962963</v>
+        <v>42137.392337962963</v>
       </c>
       <c r="C71" t="s">
         <v>30</v>
@@ -4166,7 +4211,7 @@
         <v>97</v>
       </c>
       <c r="B72" s="1">
-        <v>40675.952581018515</v>
+        <v>42137.952581018515</v>
       </c>
       <c r="C72" t="s">
         <v>30</v>
@@ -4210,7 +4255,7 @@
         <v>97</v>
       </c>
       <c r="B73" s="1">
-        <v>40676.063067129631</v>
+        <v>42138.063067129631</v>
       </c>
       <c r="C73" t="s">
         <v>30</v>
@@ -4254,7 +4299,7 @@
         <v>97</v>
       </c>
       <c r="B74" s="1">
-        <v>40676.500439814816</v>
+        <v>42138.500439814816</v>
       </c>
       <c r="C74" t="s">
         <v>30</v>
@@ -4298,7 +4343,7 @@
         <v>97</v>
       </c>
       <c r="B75" s="1">
-        <v>40677.074340277781</v>
+        <v>42139.074340277781</v>
       </c>
       <c r="C75" t="s">
         <v>30</v>
@@ -4342,7 +4387,7 @@
         <v>97</v>
       </c>
       <c r="B76" s="1">
-        <v>40677.172337962962</v>
+        <v>42139.172337962962</v>
       </c>
       <c r="C76" t="s">
         <v>30</v>
@@ -4386,7 +4431,7 @@
         <v>116</v>
       </c>
       <c r="B77" s="1">
-        <v>40648.538935185185</v>
+        <v>42110.538935185185</v>
       </c>
       <c r="C77" t="s">
         <v>117</v>
@@ -4427,7 +4472,7 @@
         <v>116</v>
       </c>
       <c r="B78" s="1">
-        <v>40648.539930555555</v>
+        <v>42110.539930555555</v>
       </c>
       <c r="C78" t="s">
         <v>117</v>
@@ -4468,7 +4513,7 @@
         <v>116</v>
       </c>
       <c r="B79" s="1">
-        <v>40648.54142361111</v>
+        <v>42110.54142361111</v>
       </c>
       <c r="C79" t="s">
         <v>117</v>
@@ -4509,7 +4554,7 @@
         <v>116</v>
       </c>
       <c r="B80" s="1">
-        <v>40648.543449074074</v>
+        <v>42110.543449074074</v>
       </c>
       <c r="C80" t="s">
         <v>117</v>
@@ -4553,7 +4598,7 @@
         <v>116</v>
       </c>
       <c r="B81" s="1">
-        <v>40648.54482638889</v>
+        <v>42110.54482638889</v>
       </c>
       <c r="C81" t="s">
         <v>117</v>
@@ -4597,7 +4642,7 @@
         <v>116</v>
       </c>
       <c r="B82" s="1">
-        <v>40648.917881944442</v>
+        <v>42110.917881944442</v>
       </c>
       <c r="C82" t="s">
         <v>117</v>
@@ -4641,7 +4686,7 @@
         <v>116</v>
       </c>
       <c r="B83" s="1">
-        <v>40648.927546296298</v>
+        <v>42110.927546296298</v>
       </c>
       <c r="C83" t="s">
         <v>117</v>
@@ -4685,7 +4730,7 @@
         <v>123</v>
       </c>
       <c r="B84" s="1">
-        <v>40651.289155092592</v>
+        <v>42113.289155092592</v>
       </c>
       <c r="C84" t="s">
         <v>124</v>
@@ -4723,7 +4768,7 @@
         <v>123</v>
       </c>
       <c r="B85" s="1">
-        <v>40651.291076388887</v>
+        <v>42113.291076388887</v>
       </c>
       <c r="C85" t="s">
         <v>124</v>
@@ -4761,7 +4806,7 @@
         <v>123</v>
       </c>
       <c r="B86" s="1">
-        <v>40651.292847222219</v>
+        <v>42113.292847222219</v>
       </c>
       <c r="C86" t="s">
         <v>124</v>
@@ -4799,7 +4844,7 @@
         <v>123</v>
       </c>
       <c r="B87" s="1">
-        <v>40651.297395833331</v>
+        <v>42113.297395833331</v>
       </c>
       <c r="C87" t="s">
         <v>124</v>
@@ -4840,7 +4885,7 @@
         <v>127</v>
       </c>
       <c r="B88" s="1">
-        <v>40641.286828703705</v>
+        <v>42103.286828703705</v>
       </c>
       <c r="C88" t="s">
         <v>128</v>
@@ -4878,7 +4923,7 @@
         <v>127</v>
       </c>
       <c r="B89" s="1">
-        <v>40641.297395833331</v>
+        <v>42103.297395833331</v>
       </c>
       <c r="C89" t="s">
         <v>128</v>
@@ -4916,7 +4961,7 @@
         <v>127</v>
       </c>
       <c r="B90" s="1">
-        <v>40641.298993055556</v>
+        <v>42103.298993055556</v>
       </c>
       <c r="C90" t="s">
         <v>128</v>
@@ -4954,7 +4999,7 @@
         <v>127</v>
       </c>
       <c r="B91" s="1">
-        <v>40641.301504629628</v>
+        <v>42103.301504629628</v>
       </c>
       <c r="C91" t="s">
         <v>128</v>
@@ -4992,7 +5037,7 @@
         <v>127</v>
       </c>
       <c r="B92" s="1">
-        <v>40641.304837962962</v>
+        <v>42103.304837962962</v>
       </c>
       <c r="C92" t="s">
         <v>128</v>
@@ -5030,7 +5075,7 @@
         <v>127</v>
       </c>
       <c r="B93" s="1">
-        <v>40641.314687500002</v>
+        <v>42103.314687500002</v>
       </c>
       <c r="C93" t="s">
         <v>128</v>
@@ -5068,7 +5113,7 @@
         <v>127</v>
       </c>
       <c r="B94" s="1">
-        <v>40641.619097222225</v>
+        <v>42103.619097222225</v>
       </c>
       <c r="C94" t="s">
         <v>128</v>
@@ -5106,7 +5151,7 @@
         <v>127</v>
       </c>
       <c r="B95" s="1">
-        <v>40641.62332175926</v>
+        <v>42103.62332175926</v>
       </c>
       <c r="C95" t="s">
         <v>128</v>
@@ -5144,7 +5189,7 @@
         <v>127</v>
       </c>
       <c r="B96" s="1">
-        <v>40641.868738425925</v>
+        <v>42103.868738425925</v>
       </c>
       <c r="C96" t="s">
         <v>128</v>
@@ -5182,7 +5227,7 @@
         <v>127</v>
       </c>
       <c r="B97" s="1">
-        <v>40641.892905092594</v>
+        <v>42103.892905092594</v>
       </c>
       <c r="C97" t="s">
         <v>128</v>
@@ -5220,7 +5265,7 @@
         <v>127</v>
       </c>
       <c r="B98" s="1">
-        <v>40641.962881944448</v>
+        <v>42103.962881944448</v>
       </c>
       <c r="C98" t="s">
         <v>128</v>
@@ -5258,7 +5303,7 @@
         <v>127</v>
       </c>
       <c r="B99" s="1">
-        <v>40647.280289351853</v>
+        <v>42109.280289351853</v>
       </c>
       <c r="C99" t="s">
         <v>128</v>
@@ -5296,7 +5341,7 @@
         <v>127</v>
       </c>
       <c r="B100" s="1">
-        <v>40647.967615740738</v>
+        <v>42109.967615740738</v>
       </c>
       <c r="C100" t="s">
         <v>128</v>
@@ -5340,7 +5385,7 @@
         <v>136</v>
       </c>
       <c r="B101" s="1">
-        <v>40654.849768518521</v>
+        <v>42116.849768518521</v>
       </c>
       <c r="C101" t="s">
         <v>128</v>
@@ -5381,7 +5426,7 @@
         <v>136</v>
       </c>
       <c r="B102" s="1">
-        <v>40654.853946759256</v>
+        <v>42116.853946759256</v>
       </c>
       <c r="C102" t="s">
         <v>128</v>
@@ -5425,7 +5470,7 @@
         <v>136</v>
       </c>
       <c r="B103" s="1">
-        <v>40654.860844907409</v>
+        <v>42116.860844907409</v>
       </c>
       <c r="C103" t="s">
         <v>128</v>
@@ -5472,7 +5517,7 @@
         <v>136</v>
       </c>
       <c r="B104" s="1">
-        <v>40654.866481481484</v>
+        <v>42116.866481481484</v>
       </c>
       <c r="C104" t="s">
         <v>128</v>
@@ -5519,7 +5564,7 @@
         <v>136</v>
       </c>
       <c r="B105" s="1">
-        <v>40654.897719907407</v>
+        <v>42116.897719907407</v>
       </c>
       <c r="C105" t="s">
         <v>128</v>
@@ -5566,7 +5611,7 @@
         <v>136</v>
       </c>
       <c r="B106" s="1">
-        <v>40655.898888888885</v>
+        <v>42117.898888888885</v>
       </c>
       <c r="C106" t="s">
         <v>128</v>
@@ -5613,7 +5658,7 @@
         <v>136</v>
       </c>
       <c r="B107" s="1">
-        <v>40656.284328703703</v>
+        <v>42118.284328703703</v>
       </c>
       <c r="C107" t="s">
         <v>140</v>
@@ -5654,7 +5699,7 @@
         <v>136</v>
       </c>
       <c r="B108" s="1">
-        <v>40656.825995370367</v>
+        <v>42118.825995370367</v>
       </c>
       <c r="C108" t="s">
         <v>140</v>
@@ -5698,7 +5743,7 @@
         <v>136</v>
       </c>
       <c r="B109" s="1">
-        <v>40656.831354166665</v>
+        <v>42118.831354166665</v>
       </c>
       <c r="C109" t="s">
         <v>140</v>
@@ -5742,7 +5787,7 @@
         <v>136</v>
       </c>
       <c r="B110" s="1">
-        <v>40656.837557870371</v>
+        <v>42118.837557870371</v>
       </c>
       <c r="C110" t="s">
         <v>140</v>
@@ -5786,7 +5831,7 @@
         <v>136</v>
       </c>
       <c r="B111" s="1">
-        <v>40656.869560185187</v>
+        <v>42118.869560185187</v>
       </c>
       <c r="C111" t="s">
         <v>140</v>
@@ -5830,7 +5875,7 @@
         <v>136</v>
       </c>
       <c r="B112" s="1">
-        <v>40656.87060185185</v>
+        <v>42118.87060185185</v>
       </c>
       <c r="C112" t="s">
         <v>140</v>
@@ -5874,7 +5919,7 @@
         <v>136</v>
       </c>
       <c r="B113" s="1">
-        <v>40656.872812499998</v>
+        <v>42118.872812499998</v>
       </c>
       <c r="C113" t="s">
         <v>140</v>
@@ -5918,7 +5963,7 @@
         <v>136</v>
       </c>
       <c r="B114" s="1">
-        <v>40656.878275462965</v>
+        <v>42118.878275462965</v>
       </c>
       <c r="C114" t="s">
         <v>140</v>
@@ -5962,7 +6007,7 @@
         <v>136</v>
       </c>
       <c r="B115" s="1">
-        <v>40656.884027777778</v>
+        <v>42118.884027777778</v>
       </c>
       <c r="C115" t="s">
         <v>140</v>
@@ -6006,7 +6051,7 @@
         <v>136</v>
       </c>
       <c r="B116" s="1">
-        <v>40656.885810185187</v>
+        <v>42118.885810185187</v>
       </c>
       <c r="C116" t="s">
         <v>140</v>
@@ -6050,7 +6095,7 @@
         <v>136</v>
       </c>
       <c r="B117" s="1">
-        <v>40656.890127314815</v>
+        <v>42118.890127314815</v>
       </c>
       <c r="C117" t="s">
         <v>140</v>
@@ -6094,7 +6139,7 @@
         <v>136</v>
       </c>
       <c r="B118" s="1">
-        <v>40656.894976851851</v>
+        <v>42118.894976851851</v>
       </c>
       <c r="C118" t="s">
         <v>140</v>
@@ -6138,7 +6183,7 @@
         <v>136</v>
       </c>
       <c r="B119" s="1">
-        <v>40656.899618055555</v>
+        <v>42118.899618055555</v>
       </c>
       <c r="C119" t="s">
         <v>140</v>
@@ -6182,7 +6227,7 @@
         <v>136</v>
       </c>
       <c r="B120" s="1">
-        <v>40656.904513888891</v>
+        <v>42118.904513888891</v>
       </c>
       <c r="C120" t="s">
         <v>140</v>
@@ -6226,7 +6271,7 @@
         <v>136</v>
       </c>
       <c r="B121" s="1">
-        <v>40666.813668981478</v>
+        <v>42128.813668981478</v>
       </c>
       <c r="C121" t="s">
         <v>140</v>
@@ -6270,7 +6315,7 @@
         <v>136</v>
       </c>
       <c r="B122" s="1">
-        <v>40666.822210648148</v>
+        <v>42128.822210648148</v>
       </c>
       <c r="C122" t="s">
         <v>140</v>
@@ -6314,7 +6359,7 @@
         <v>136</v>
       </c>
       <c r="B123" s="1">
-        <v>40666.829050925924</v>
+        <v>42128.829050925924</v>
       </c>
       <c r="C123" t="s">
         <v>140</v>
@@ -6358,7 +6403,7 @@
         <v>136</v>
       </c>
       <c r="B124" s="1">
-        <v>40666.858576388891</v>
+        <v>42128.858576388891</v>
       </c>
       <c r="C124" t="s">
         <v>140</v>
@@ -6402,7 +6447,7 @@
         <v>136</v>
       </c>
       <c r="B125" s="1">
-        <v>40666.864722222221</v>
+        <v>42128.864722222221</v>
       </c>
       <c r="C125" t="s">
         <v>140</v>
@@ -6446,7 +6491,7 @@
         <v>136</v>
       </c>
       <c r="B126" s="1">
-        <v>40666.87090277778</v>
+        <v>42128.87090277778</v>
       </c>
       <c r="C126" t="s">
         <v>140</v>
@@ -6490,7 +6535,7 @@
         <v>165</v>
       </c>
       <c r="B127" s="1">
-        <v>40658.815578703703</v>
+        <v>42120.815578703703</v>
       </c>
       <c r="C127" t="s">
         <v>128</v>
@@ -6534,7 +6579,7 @@
         <v>165</v>
       </c>
       <c r="B128" s="1">
-        <v>40658.824513888889</v>
+        <v>42120.824513888889</v>
       </c>
       <c r="C128" t="s">
         <v>128</v>
@@ -6578,7 +6623,7 @@
         <v>165</v>
       </c>
       <c r="B129" s="1">
-        <v>40658.838333333333</v>
+        <v>42120.838333333333</v>
       </c>
       <c r="C129" t="s">
         <v>128</v>
@@ -6622,7 +6667,7 @@
         <v>165</v>
       </c>
       <c r="B130" s="1">
-        <v>40658.874039351853</v>
+        <v>42120.874039351853</v>
       </c>
       <c r="C130" t="s">
         <v>128</v>
@@ -6666,7 +6711,7 @@
         <v>165</v>
       </c>
       <c r="B131" s="1">
-        <v>40658.947094907409</v>
+        <v>42120.947094907409</v>
       </c>
       <c r="C131" t="s">
         <v>128</v>
@@ -6710,7 +6755,7 @@
         <v>173</v>
       </c>
       <c r="B132" s="1">
-        <v>40699.796435185184</v>
+        <v>42161.796435185184</v>
       </c>
       <c r="C132" t="s">
         <v>174</v>
@@ -6748,7 +6793,7 @@
         <v>173</v>
       </c>
       <c r="B133" s="1">
-        <v>40699.934270833335</v>
+        <v>42161.934270833335</v>
       </c>
       <c r="C133" t="s">
         <v>174</v>
@@ -6786,7 +6831,7 @@
         <v>173</v>
       </c>
       <c r="B134" s="1">
-        <v>40699.951678240737</v>
+        <v>42161.951678240737</v>
       </c>
       <c r="C134" t="s">
         <v>174</v>
@@ -6824,7 +6869,7 @@
         <v>173</v>
       </c>
       <c r="B135" s="1">
-        <v>40700.261076388888</v>
+        <v>42162.261076388888</v>
       </c>
       <c r="C135" t="s">
         <v>174</v>
@@ -6859,46 +6904,40 @@
     </row>
     <row r="136" spans="1:15">
       <c r="A136" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B136" s="1">
-        <v>40699.592685185184</v>
+        <v>42162.667824074073</v>
       </c>
       <c r="C136" t="s">
-        <v>30</v>
+        <v>174</v>
       </c>
       <c r="D136">
-        <v>853.95600000000002</v>
+        <v>11.6619999999999</v>
       </c>
       <c r="E136">
-        <v>11.973000000000001</v>
+        <v>5.7999999999999802E-2</v>
       </c>
       <c r="F136">
-        <v>301.11500000000001</v>
+        <v>11.712999999999701</v>
       </c>
       <c r="G136">
-        <v>5573</v>
+        <v>0</v>
       </c>
       <c r="H136">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="I136">
-        <v>0.66626236129503302</v>
+        <v>0.54210109176232901</v>
       </c>
       <c r="J136" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K136" t="s">
-        <v>180</v>
-      </c>
-      <c r="M136" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="N136" t="s">
-        <v>181</v>
-      </c>
-      <c r="O136" t="s">
-        <v>20</v>
+        <v>176</v>
       </c>
     </row>
     <row r="137" spans="1:15">
@@ -6906,34 +6945,34 @@
         <v>179</v>
       </c>
       <c r="B137" s="1">
-        <v>40699.861921296295</v>
+        <v>42161.592685185184</v>
       </c>
       <c r="C137" t="s">
         <v>30</v>
       </c>
       <c r="D137">
-        <v>2765.0250000000001</v>
+        <v>853.95600000000002</v>
       </c>
       <c r="E137">
-        <v>29.762</v>
+        <v>11.973000000000001</v>
       </c>
       <c r="F137">
-        <v>776.72</v>
+        <v>301.11500000000001</v>
       </c>
       <c r="G137">
-        <v>13927</v>
+        <v>5573</v>
       </c>
       <c r="H137">
         <v>94</v>
       </c>
       <c r="I137">
-        <v>0.623107636466533</v>
+        <v>0.66626236129503302</v>
       </c>
       <c r="J137" t="s">
         <v>17</v>
       </c>
       <c r="K137" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M137" t="s">
         <v>40</v>
@@ -6947,46 +6986,46 @@
     </row>
     <row r="138" spans="1:15">
       <c r="A138" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B138" s="1">
-        <v>40699.707442129627</v>
+        <v>42161.861921296295</v>
       </c>
       <c r="C138" t="s">
         <v>30</v>
       </c>
       <c r="D138">
-        <v>1177.08</v>
+        <v>2765.0250000000001</v>
       </c>
       <c r="E138">
-        <v>17.669</v>
+        <v>29.762</v>
       </c>
       <c r="F138">
-        <v>331.49</v>
+        <v>776.72</v>
       </c>
       <c r="G138">
-        <v>5573</v>
+        <v>13927</v>
       </c>
       <c r="H138">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="I138">
-        <v>0.60818851565530396</v>
+        <v>0.623107636466533</v>
       </c>
       <c r="J138" t="s">
         <v>17</v>
       </c>
       <c r="K138" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M138" t="s">
         <v>40</v>
       </c>
       <c r="N138" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="O138" t="s">
-        <v>186</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:15">
@@ -6994,34 +7033,34 @@
         <v>183</v>
       </c>
       <c r="B139" s="1">
-        <v>40699.930277777778</v>
+        <v>42161.707442129627</v>
       </c>
       <c r="C139" t="s">
         <v>30</v>
       </c>
       <c r="D139">
-        <v>17341.705000000002</v>
+        <v>1177.08</v>
       </c>
       <c r="E139">
-        <v>124.589</v>
+        <v>17.669</v>
       </c>
       <c r="F139">
-        <v>4701.299</v>
+        <v>331.49</v>
       </c>
       <c r="G139">
-        <v>13926</v>
+        <v>5573</v>
       </c>
       <c r="H139">
         <v>112</v>
       </c>
       <c r="I139">
-        <v>0.56554001799711895</v>
+        <v>0.60818851565530396</v>
       </c>
       <c r="J139" t="s">
         <v>17</v>
       </c>
       <c r="K139" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="M139" t="s">
         <v>40</v>
@@ -7038,19 +7077,19 @@
         <v>183</v>
       </c>
       <c r="B140" s="1">
-        <v>40700.244930555556</v>
+        <v>42161.930277777778</v>
       </c>
       <c r="C140" t="s">
         <v>30</v>
       </c>
       <c r="D140">
-        <v>2509.1959999999999</v>
+        <v>17341.705000000002</v>
       </c>
       <c r="E140">
-        <v>27.016999999999999</v>
+        <v>124.589</v>
       </c>
       <c r="F140">
-        <v>865.4</v>
+        <v>4701.299</v>
       </c>
       <c r="G140">
         <v>13926</v>
@@ -7059,13 +7098,13 @@
         <v>112</v>
       </c>
       <c r="I140">
-        <v>0.55931398293880896</v>
+        <v>0.56554001799711895</v>
       </c>
       <c r="J140" t="s">
         <v>17</v>
       </c>
       <c r="K140" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M140" t="s">
         <v>40</v>
@@ -7079,510 +7118,576 @@
     </row>
     <row r="141" spans="1:15">
       <c r="A141" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B141" s="1">
-        <v>40699.571192129632</v>
+        <v>42162.244930555556</v>
       </c>
       <c r="C141" t="s">
-        <v>128</v>
+        <v>30</v>
       </c>
       <c r="D141">
-        <v>871.49900000000002</v>
+        <v>2509.1959999999999</v>
       </c>
       <c r="E141">
-        <v>8.6029999999999998</v>
+        <v>27.016999999999999</v>
       </c>
       <c r="F141">
-        <v>241.07300000000001</v>
+        <v>865.4</v>
       </c>
       <c r="G141">
-        <v>5573</v>
+        <v>13926</v>
       </c>
       <c r="H141">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="I141">
-        <v>0.68809918722022201</v>
+        <v>0.55931398293880896</v>
       </c>
       <c r="J141" t="s">
         <v>17</v>
       </c>
       <c r="K141" t="s">
-        <v>137</v>
+        <v>188</v>
       </c>
       <c r="M141" t="s">
-        <v>131</v>
+        <v>40</v>
+      </c>
+      <c r="N141" t="s">
+        <v>185</v>
       </c>
       <c r="O141" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="142" spans="1:15">
       <c r="A142" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B142" s="1">
-        <v>40699.850671296299</v>
+        <v>42162.626851851855</v>
       </c>
       <c r="C142" t="s">
-        <v>128</v>
+        <v>30</v>
       </c>
       <c r="D142">
-        <v>2617.5419999999999</v>
+        <v>2790.47</v>
       </c>
       <c r="E142">
-        <v>22.308</v>
+        <v>29.757000000000001</v>
       </c>
       <c r="F142">
-        <v>818.97400000000005</v>
+        <v>911.73700000000099</v>
       </c>
       <c r="G142">
-        <v>13927</v>
+        <v>13926</v>
       </c>
       <c r="H142">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="I142">
-        <v>0.62943452506077502</v>
+        <v>0.55557532293027601</v>
       </c>
       <c r="J142" t="s">
         <v>17</v>
       </c>
       <c r="K142" t="s">
-        <v>137</v>
+        <v>189</v>
       </c>
       <c r="M142" t="s">
-        <v>131</v>
+        <v>40</v>
+      </c>
+      <c r="N142" t="s">
+        <v>185</v>
       </c>
       <c r="O142" t="s">
-        <v>20</v>
+        <v>190</v>
       </c>
     </row>
     <row r="143" spans="1:15">
       <c r="A143" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B143" s="1">
-        <v>40699.695405092592</v>
+        <v>42162.543749999997</v>
       </c>
       <c r="C143" t="s">
-        <v>128</v>
+        <v>30</v>
       </c>
       <c r="D143">
-        <v>972.75899999999899</v>
+        <v>2132.36</v>
       </c>
       <c r="E143">
-        <v>9.8089999999999993</v>
+        <v>22.695</v>
       </c>
       <c r="F143">
-        <v>246.960000000001</v>
+        <v>761.02200000000005</v>
       </c>
       <c r="G143">
-        <v>5573</v>
+        <v>13927</v>
       </c>
       <c r="H143">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="I143">
-        <v>0.66506875332002702</v>
+        <v>0.62151911209008603</v>
       </c>
       <c r="J143" t="s">
         <v>17</v>
       </c>
       <c r="K143" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M143" t="s">
-        <v>131</v>
+        <v>40</v>
       </c>
       <c r="N143" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="O143" t="s">
-        <v>186</v>
+        <v>20</v>
       </c>
     </row>
     <row r="144" spans="1:15">
       <c r="A144" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B144" s="1">
-        <v>40699.868159722224</v>
+        <v>42162.553344907406</v>
       </c>
       <c r="C144" t="s">
-        <v>128</v>
+        <v>30</v>
       </c>
       <c r="D144">
-        <v>206.69200000000001</v>
+        <v>2150.2109999999998</v>
       </c>
       <c r="E144">
-        <v>0.64200000000000002</v>
+        <v>25.023</v>
       </c>
       <c r="F144">
-        <v>207.304</v>
+        <v>740.88699999999994</v>
       </c>
       <c r="G144">
-        <v>13926</v>
+        <v>13927</v>
       </c>
       <c r="H144">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="I144">
-        <v>0.62311786296301297</v>
+        <v>0.62559520441015104</v>
       </c>
       <c r="J144" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K144" t="s">
-        <v>191</v>
-      </c>
-      <c r="L144" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="M144" t="s">
-        <v>131</v>
+        <v>195</v>
       </c>
       <c r="N144" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="O144" t="s">
-        <v>186</v>
+        <v>20</v>
       </c>
     </row>
     <row r="145" spans="1:15">
       <c r="A145" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B145" s="1">
-        <v>40642.007476851853</v>
+        <v>42162.563090277778</v>
       </c>
       <c r="C145" t="s">
-        <v>194</v>
+        <v>30</v>
       </c>
       <c r="D145">
-        <v>315.97500000000002</v>
+        <v>2164.366</v>
       </c>
       <c r="E145">
-        <v>29.097000000000001</v>
+        <v>23.768999999999998</v>
       </c>
       <c r="F145">
-        <v>323.35300000000001</v>
+        <v>756.34500000000003</v>
       </c>
       <c r="G145">
-        <v>7426</v>
+        <v>13927</v>
       </c>
       <c r="H145">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="I145">
-        <v>1.59003529389746</v>
+        <v>0.61301514600863105</v>
+      </c>
+      <c r="J145" t="s">
+        <v>17</v>
       </c>
       <c r="K145" t="s">
-        <v>195</v>
+        <v>197</v>
+      </c>
+      <c r="M145" t="s">
+        <v>198</v>
+      </c>
+      <c r="N145" t="s">
+        <v>199</v>
       </c>
       <c r="O145" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="146" spans="1:15">
       <c r="A146" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B146" s="1">
-        <v>40644.830034722225</v>
+        <v>42162.574155092596</v>
       </c>
       <c r="C146" t="s">
-        <v>196</v>
+        <v>30</v>
       </c>
       <c r="D146">
-        <v>72.912000000000006</v>
+        <v>2176.8040000000001</v>
       </c>
       <c r="E146">
-        <v>2.387</v>
+        <v>24.056999999999999</v>
       </c>
       <c r="F146">
-        <v>74.873000000000005</v>
+        <v>759.88499999999999</v>
       </c>
       <c r="G146">
-        <v>7426</v>
+        <v>13927</v>
       </c>
       <c r="H146">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="I146">
-        <v>1.58129073532396</v>
+        <v>0.61792130927522304</v>
+      </c>
+      <c r="J146" t="s">
+        <v>21</v>
       </c>
       <c r="K146" t="s">
-        <v>197</v>
+        <v>200</v>
+      </c>
+      <c r="M146" t="s">
+        <v>201</v>
+      </c>
+      <c r="N146" t="s">
+        <v>202</v>
       </c>
       <c r="O146" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="147" spans="1:15">
       <c r="A147" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="B147" s="1">
-        <v>40644.84652777778</v>
+        <v>42161.571192129632</v>
       </c>
       <c r="C147" t="s">
-        <v>196</v>
+        <v>128</v>
       </c>
       <c r="D147">
-        <v>15.842000000000001</v>
+        <v>871.49900000000002</v>
       </c>
       <c r="E147">
-        <v>0.49100000000000099</v>
+        <v>8.6029999999999998</v>
       </c>
       <c r="F147">
-        <v>36.243999999999701</v>
+        <v>241.07300000000001</v>
       </c>
       <c r="G147">
-        <v>7426</v>
+        <v>5573</v>
       </c>
       <c r="H147">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="I147">
-        <v>1.5374895271743101</v>
+        <v>0.68809918722022201</v>
+      </c>
+      <c r="J147" t="s">
+        <v>17</v>
       </c>
       <c r="K147" t="s">
-        <v>197</v>
+        <v>137</v>
+      </c>
+      <c r="M147" t="s">
+        <v>131</v>
       </c>
       <c r="O147" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="148" spans="1:15">
       <c r="A148" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="B148" s="1">
-        <v>40644.848807870374</v>
+        <v>42161.850671296299</v>
       </c>
       <c r="C148" t="s">
-        <v>196</v>
+        <v>128</v>
       </c>
       <c r="D148">
-        <v>15.901</v>
+        <v>2617.5419999999999</v>
       </c>
       <c r="E148">
-        <v>0.44700000000000101</v>
+        <v>22.308</v>
       </c>
       <c r="F148">
-        <v>36.188000000000102</v>
+        <v>818.97400000000005</v>
       </c>
       <c r="G148">
-        <v>7426</v>
+        <v>13927</v>
       </c>
       <c r="H148">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="I148">
-        <v>1.5374895271743101</v>
+        <v>0.62943452506077502</v>
+      </c>
+      <c r="J148" t="s">
+        <v>17</v>
       </c>
       <c r="K148" t="s">
-        <v>197</v>
+        <v>137</v>
+      </c>
+      <c r="M148" t="s">
+        <v>131</v>
       </c>
       <c r="O148" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="149" spans="1:15">
       <c r="A149" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B149" s="1">
-        <v>40644.853368055556</v>
+        <v>42161.695405092592</v>
       </c>
       <c r="C149" t="s">
-        <v>196</v>
+        <v>128</v>
       </c>
       <c r="D149">
-        <v>15.009</v>
+        <v>972.75899999999899</v>
       </c>
       <c r="E149">
-        <v>0.57799999999999896</v>
+        <v>9.8089999999999993</v>
       </c>
       <c r="F149">
-        <v>114.17400000000001</v>
+        <v>246.960000000001</v>
       </c>
       <c r="G149">
-        <v>7426</v>
+        <v>5573</v>
       </c>
       <c r="H149">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="I149">
-        <v>1.5939681680293001</v>
+        <v>0.66506875332002702</v>
+      </c>
+      <c r="J149" t="s">
+        <v>17</v>
       </c>
       <c r="K149" t="s">
-        <v>198</v>
+        <v>205</v>
+      </c>
+      <c r="M149" t="s">
+        <v>131</v>
+      </c>
+      <c r="N149" t="s">
+        <v>206</v>
       </c>
       <c r="O149" t="s">
-        <v>32</v>
+        <v>186</v>
       </c>
     </row>
     <row r="150" spans="1:15">
       <c r="A150" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B150" s="1">
-        <v>40644.856076388889</v>
+        <v>42161.868159722224</v>
       </c>
       <c r="C150" t="s">
-        <v>196</v>
+        <v>128</v>
       </c>
       <c r="D150">
-        <v>15.125</v>
+        <v>206.69200000000001</v>
       </c>
       <c r="E150">
-        <v>0.54299999999999904</v>
+        <v>0.64200000000000002</v>
       </c>
       <c r="F150">
-        <v>116.895</v>
+        <v>207.304</v>
       </c>
       <c r="G150">
-        <v>7426</v>
+        <v>13926</v>
       </c>
       <c r="H150">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="I150">
-        <v>1.5939681680293001</v>
+        <v>0.62311786296301297</v>
+      </c>
+      <c r="J150" t="s">
+        <v>17</v>
       </c>
       <c r="K150" t="s">
-        <v>198</v>
+        <v>205</v>
+      </c>
+      <c r="L150" t="s">
+        <v>205</v>
+      </c>
+      <c r="M150" t="s">
+        <v>131</v>
+      </c>
+      <c r="N150" t="s">
+        <v>206</v>
       </c>
       <c r="O150" t="s">
-        <v>32</v>
+        <v>186</v>
       </c>
     </row>
     <row r="151" spans="1:15">
       <c r="A151" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B151" s="1">
-        <v>40644.859270833331</v>
+        <v>42162.614976851852</v>
       </c>
       <c r="C151" t="s">
-        <v>196</v>
+        <v>128</v>
       </c>
       <c r="D151">
-        <v>14.928000000000001</v>
+        <v>238.864</v>
       </c>
       <c r="E151">
-        <v>0.40100000000000002</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="F151">
-        <v>15.249000000000301</v>
+        <v>239.37900000000101</v>
       </c>
       <c r="G151">
-        <v>7426</v>
+        <v>13926</v>
       </c>
       <c r="H151">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="I151">
-        <v>1.57773355605539</v>
+        <v>0.56686356751435596</v>
+      </c>
+      <c r="J151" t="s">
+        <v>17</v>
       </c>
       <c r="K151" t="s">
-        <v>198</v>
+        <v>207</v>
+      </c>
+      <c r="L151" t="s">
+        <v>207</v>
+      </c>
+      <c r="M151" t="s">
+        <v>131</v>
+      </c>
+      <c r="N151" t="s">
+        <v>206</v>
       </c>
       <c r="O151" t="s">
-        <v>32</v>
+        <v>190</v>
       </c>
     </row>
     <row r="152" spans="1:15">
       <c r="A152" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B152" s="1">
-        <v>40644.861122685186</v>
+        <v>42104.007476851853</v>
       </c>
       <c r="C152" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="D152">
-        <v>16.733000000000001</v>
+        <v>315.97500000000002</v>
       </c>
       <c r="E152">
-        <v>0.47099999999999997</v>
+        <v>29.097000000000001</v>
       </c>
       <c r="F152">
-        <v>17.1170000000002</v>
+        <v>323.35300000000001</v>
       </c>
       <c r="G152">
         <v>7426</v>
       </c>
       <c r="H152">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I152">
-        <v>1.56821048218277</v>
+        <v>1.59003529389746</v>
       </c>
       <c r="K152" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="O152" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="153" spans="1:15">
       <c r="A153" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B153" s="1">
-        <v>40644.862372685187</v>
+        <v>42106.830034722225</v>
       </c>
       <c r="C153" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D153">
-        <v>17.763000000000002</v>
+        <v>72.912000000000006</v>
       </c>
       <c r="E153">
-        <v>0.49</v>
+        <v>2.387</v>
       </c>
       <c r="F153">
-        <v>18.158000000000399</v>
+        <v>74.873000000000005</v>
       </c>
       <c r="G153">
         <v>7426</v>
       </c>
       <c r="H153">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I153">
-        <v>1.6500830141598</v>
+        <v>1.58129073532396</v>
       </c>
       <c r="K153" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="O153" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="154" spans="1:15">
       <c r="A154" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B154" s="1">
-        <v>40644.863437499997</v>
+        <v>42106.84652777778</v>
       </c>
       <c r="C154" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D154">
-        <v>15.666</v>
+        <v>15.842000000000001</v>
       </c>
       <c r="E154">
-        <v>0.47699999999999998</v>
+        <v>0.49100000000000099</v>
       </c>
       <c r="F154">
-        <v>16.0569999999998</v>
+        <v>36.243999999999701</v>
       </c>
       <c r="G154">
         <v>7426</v>
@@ -7591,10 +7696,10 @@
         <v>80</v>
       </c>
       <c r="I154">
-        <v>1.54316586262694</v>
+        <v>1.5374895271743101</v>
       </c>
       <c r="K154" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="O154" t="s">
         <v>32</v>
@@ -7602,34 +7707,34 @@
     </row>
     <row r="155" spans="1:15">
       <c r="A155" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B155" s="1">
-        <v>40644.868576388886</v>
+        <v>42106.848807870374</v>
       </c>
       <c r="C155" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D155">
-        <v>54.494999999999997</v>
+        <v>15.901</v>
       </c>
       <c r="E155">
-        <v>1.0149999999999999</v>
+        <v>0.44700000000000101</v>
       </c>
       <c r="F155">
-        <v>55.336000000000197</v>
+        <v>36.188000000000102</v>
       </c>
       <c r="G155">
-        <v>14852</v>
+        <v>7426</v>
       </c>
       <c r="H155">
         <v>80</v>
       </c>
       <c r="I155">
-        <v>1.8013924389029601</v>
+        <v>1.5374895271743101</v>
       </c>
       <c r="K155" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="O155" t="s">
         <v>32</v>
@@ -7637,34 +7742,34 @@
     </row>
     <row r="156" spans="1:15">
       <c r="A156" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B156" s="1">
-        <v>40644.876087962963</v>
+        <v>42106.853368055556</v>
       </c>
       <c r="C156" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D156">
-        <v>46.767000000000102</v>
+        <v>15.009</v>
       </c>
       <c r="E156">
-        <v>1.6379999999999999</v>
+        <v>0.57799999999999896</v>
       </c>
       <c r="F156">
-        <v>553.19600000000003</v>
+        <v>114.17400000000001</v>
       </c>
       <c r="G156">
-        <v>14852</v>
+        <v>7426</v>
       </c>
       <c r="H156">
         <v>80</v>
       </c>
       <c r="I156">
-        <v>1.6284161515828499</v>
+        <v>1.5939681680293001</v>
       </c>
       <c r="K156" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="O156" t="s">
         <v>32</v>
@@ -7672,34 +7777,34 @@
     </row>
     <row r="157" spans="1:15">
       <c r="A157" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B157" s="1">
-        <v>40644.890833333331</v>
+        <v>42106.856076388889</v>
       </c>
       <c r="C157" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D157">
-        <v>94.869</v>
+        <v>15.125</v>
       </c>
       <c r="E157">
-        <v>3.2869999999999999</v>
+        <v>0.54299999999999904</v>
       </c>
       <c r="F157">
-        <v>1216.4549999999999</v>
+        <v>116.895</v>
       </c>
       <c r="G157">
-        <v>22278</v>
+        <v>7426</v>
       </c>
       <c r="H157">
         <v>80</v>
       </c>
       <c r="I157">
-        <v>1.58337486055827</v>
+        <v>1.5939681680293001</v>
       </c>
       <c r="K157" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="O157" t="s">
         <v>32</v>
@@ -7707,34 +7812,34 @@
     </row>
     <row r="158" spans="1:15">
       <c r="A158" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B158" s="1">
-        <v>40644.980844907404</v>
+        <v>42106.859270833331</v>
       </c>
       <c r="C158" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D158">
-        <v>95.006</v>
+        <v>14.928000000000001</v>
       </c>
       <c r="E158">
-        <v>3.335</v>
+        <v>0.40100000000000002</v>
       </c>
       <c r="F158">
-        <v>1510.02</v>
+        <v>15.249000000000301</v>
       </c>
       <c r="G158">
-        <v>22278</v>
+        <v>7426</v>
       </c>
       <c r="H158">
         <v>80</v>
       </c>
       <c r="I158">
-        <v>1.5833199935014</v>
+        <v>1.57773355605539</v>
       </c>
       <c r="K158" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="O158" t="s">
         <v>32</v>
@@ -7742,104 +7847,104 @@
     </row>
     <row r="159" spans="1:15">
       <c r="A159" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B159" s="1">
-        <v>40645.289965277778</v>
+        <v>42106.861122685186</v>
       </c>
       <c r="C159" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D159">
-        <v>126.211</v>
+        <v>16.733000000000001</v>
       </c>
       <c r="E159">
-        <v>1.462</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="F159">
-        <v>127.443</v>
+        <v>17.1170000000002</v>
       </c>
       <c r="G159">
-        <v>22278</v>
+        <v>7426</v>
       </c>
       <c r="H159">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="I159">
-        <v>1.92982759815376</v>
+        <v>1.56821048218277</v>
       </c>
       <c r="K159" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="O159" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="160" spans="1:15">
       <c r="A160" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B160" s="1">
-        <v>40645.295682870368</v>
+        <v>42106.862372685187</v>
       </c>
       <c r="C160" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D160">
-        <v>91.376999999999995</v>
+        <v>17.763000000000002</v>
       </c>
       <c r="E160">
-        <v>1.498</v>
+        <v>0.49</v>
       </c>
       <c r="F160">
-        <v>92.478999999999999</v>
+        <v>18.158000000000399</v>
       </c>
       <c r="G160">
-        <v>22278</v>
+        <v>7426</v>
       </c>
       <c r="H160">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="I160">
-        <v>1.58384242553734</v>
+        <v>1.6500830141598</v>
       </c>
       <c r="K160" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="O160" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="161" spans="1:15">
       <c r="A161" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B161" s="1">
-        <v>40645.301527777781</v>
+        <v>42106.863437499997</v>
       </c>
       <c r="C161" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D161">
-        <v>230.64400000000001</v>
+        <v>15.666</v>
       </c>
       <c r="E161">
-        <v>3.0230000000000001</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="F161">
-        <v>232.80799999999999</v>
+        <v>16.0569999999998</v>
       </c>
       <c r="G161">
-        <v>37131</v>
+        <v>7426</v>
       </c>
       <c r="H161">
         <v>80</v>
       </c>
       <c r="I161">
-        <v>1.60920568515367</v>
+        <v>1.54316586262694</v>
       </c>
       <c r="K161" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="O161" t="s">
         <v>32</v>
@@ -7847,43 +7952,34 @@
     </row>
     <row r="162" spans="1:15">
       <c r="A162" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B162" s="1">
-        <v>40647.907395833332</v>
+        <v>42106.868576388886</v>
       </c>
       <c r="C162" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D162">
-        <v>12.09</v>
+        <v>54.494999999999997</v>
       </c>
       <c r="E162">
-        <v>0.53400000000000003</v>
+        <v>1.0149999999999999</v>
       </c>
       <c r="F162">
-        <v>12.579999999999901</v>
+        <v>55.336000000000197</v>
       </c>
       <c r="G162">
-        <v>1856</v>
+        <v>14852</v>
       </c>
       <c r="H162">
         <v>80</v>
       </c>
       <c r="I162">
-        <v>1.66250101299196</v>
-      </c>
-      <c r="J162" t="s">
-        <v>21</v>
+        <v>1.8013924389029601</v>
       </c>
       <c r="K162" t="s">
-        <v>199</v>
-      </c>
-      <c r="L162" t="s">
-        <v>200</v>
-      </c>
-      <c r="M162" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="O162" t="s">
         <v>32</v>
@@ -7891,43 +7987,34 @@
     </row>
     <row r="163" spans="1:15">
       <c r="A163" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B163" s="1">
-        <v>40647.90828703704</v>
+        <v>42106.876087962963</v>
       </c>
       <c r="C163" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D163">
-        <v>20.206</v>
+        <v>46.767000000000102</v>
       </c>
       <c r="E163">
-        <v>1.0740000000000001</v>
+        <v>1.6379999999999999</v>
       </c>
       <c r="F163">
-        <v>21.203000000000401</v>
+        <v>553.19600000000003</v>
       </c>
       <c r="G163">
-        <v>1856</v>
+        <v>14852</v>
       </c>
       <c r="H163">
         <v>80</v>
       </c>
       <c r="I163">
-        <v>1.63488299912919</v>
-      </c>
-      <c r="J163" t="s">
-        <v>21</v>
+        <v>1.6284161515828499</v>
       </c>
       <c r="K163" t="s">
-        <v>202</v>
-      </c>
-      <c r="L163" t="s">
-        <v>203</v>
-      </c>
-      <c r="M163" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="O163" t="s">
         <v>32</v>
@@ -7935,43 +8022,34 @@
     </row>
     <row r="164" spans="1:15">
       <c r="A164" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B164" s="1">
-        <v>40647.910219907404</v>
+        <v>42106.890833333331</v>
       </c>
       <c r="C164" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D164">
-        <v>20.748999999999999</v>
+        <v>94.869</v>
       </c>
       <c r="E164">
-        <v>1.0349999999999999</v>
+        <v>3.2869999999999999</v>
       </c>
       <c r="F164">
-        <v>21.721999999999799</v>
+        <v>1216.4549999999999</v>
       </c>
       <c r="G164">
-        <v>1856</v>
+        <v>22278</v>
       </c>
       <c r="H164">
         <v>80</v>
       </c>
       <c r="I164">
-        <v>1</v>
-      </c>
-      <c r="J164" t="s">
-        <v>17</v>
+        <v>1.58337486055827</v>
       </c>
       <c r="K164" t="s">
-        <v>202</v>
-      </c>
-      <c r="L164" t="s">
-        <v>203</v>
-      </c>
-      <c r="M164" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="O164" t="s">
         <v>32</v>
@@ -7979,43 +8057,34 @@
     </row>
     <row r="165" spans="1:15">
       <c r="A165" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B165" s="1">
-        <v>40647.911585648151</v>
+        <v>42106.980844907404</v>
       </c>
       <c r="C165" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D165">
-        <v>20.614000000000001</v>
+        <v>95.006</v>
       </c>
       <c r="E165">
-        <v>1.004</v>
+        <v>3.335</v>
       </c>
       <c r="F165">
-        <v>21.542999999999701</v>
+        <v>1510.02</v>
       </c>
       <c r="G165">
-        <v>1856</v>
+        <v>22278</v>
       </c>
       <c r="H165">
         <v>80</v>
       </c>
       <c r="I165">
-        <v>0.99</v>
-      </c>
-      <c r="J165" t="s">
-        <v>17</v>
+        <v>1.5833199935014</v>
       </c>
       <c r="K165" t="s">
-        <v>202</v>
-      </c>
-      <c r="L165" t="s">
-        <v>203</v>
-      </c>
-      <c r="M165" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="O165" t="s">
         <v>32</v>
@@ -8023,43 +8092,34 @@
     </row>
     <row r="166" spans="1:15">
       <c r="A166" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B166" s="1">
-        <v>40647.918564814812</v>
+        <v>42107.289965277778</v>
       </c>
       <c r="C166" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D166">
-        <v>20.510999999999999</v>
+        <v>126.211</v>
       </c>
       <c r="E166">
-        <v>1.0049999999999999</v>
+        <v>1.462</v>
       </c>
       <c r="F166">
-        <v>21.440000000000499</v>
+        <v>127.443</v>
       </c>
       <c r="G166">
-        <v>1856</v>
+        <v>22278</v>
       </c>
       <c r="H166">
         <v>80</v>
       </c>
       <c r="I166">
-        <v>1.63488299912919</v>
-      </c>
-      <c r="J166" t="s">
-        <v>21</v>
+        <v>1.92982759815376</v>
       </c>
       <c r="K166" t="s">
-        <v>202</v>
-      </c>
-      <c r="L166" t="s">
-        <v>203</v>
-      </c>
-      <c r="M166" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="O166" t="s">
         <v>32</v>
@@ -8067,40 +8127,34 @@
     </row>
     <row r="167" spans="1:15">
       <c r="A167" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B167" s="1">
-        <v>40659.844583333332</v>
+        <v>42107.295682870368</v>
       </c>
       <c r="C167" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D167">
-        <v>3.0630000000000002</v>
+        <v>91.376999999999995</v>
       </c>
       <c r="E167">
-        <v>0.26600000000000001</v>
+        <v>1.498</v>
       </c>
       <c r="F167">
-        <v>93.864000000000502</v>
+        <v>92.478999999999999</v>
       </c>
       <c r="G167">
-        <v>1856</v>
+        <v>22278</v>
       </c>
       <c r="H167">
         <v>80</v>
       </c>
       <c r="I167">
-        <v>1.6325571524315501</v>
-      </c>
-      <c r="J167" t="s">
-        <v>21</v>
+        <v>1.58384242553734</v>
       </c>
       <c r="K167" t="s">
-        <v>205</v>
-      </c>
-      <c r="N167" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="O167" t="s">
         <v>32</v>
@@ -8108,339 +8162,336 @@
     </row>
     <row r="168" spans="1:15">
       <c r="A168" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B168" s="1">
-        <v>40659.847118055557</v>
+        <v>42107.301527777781</v>
       </c>
       <c r="C168" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D168">
-        <v>2.976</v>
+        <v>230.64400000000001</v>
       </c>
       <c r="E168">
-        <v>0.28299999999999997</v>
+        <v>3.0230000000000001</v>
       </c>
       <c r="F168">
-        <v>100.997</v>
+        <v>232.80799999999999</v>
       </c>
       <c r="G168">
-        <v>1856</v>
+        <v>37131</v>
       </c>
       <c r="H168">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I168">
-        <v>1.5866800350352499</v>
-      </c>
-      <c r="J168" t="s">
-        <v>21</v>
+        <v>1.60920568515367</v>
       </c>
       <c r="K168" t="s">
-        <v>207</v>
-      </c>
-      <c r="N168" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="O168" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="169" spans="1:15">
       <c r="A169" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B169" s="1">
-        <v>40659.848344907405</v>
+        <v>42109.907395833332</v>
       </c>
       <c r="C169" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D169">
-        <v>2.48</v>
+        <v>12.09</v>
       </c>
       <c r="E169">
-        <v>0.13899999999999901</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="F169">
-        <v>9.2620000000006293</v>
+        <v>12.579999999999901</v>
       </c>
       <c r="G169">
         <v>1856</v>
       </c>
       <c r="H169">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I169">
-        <v>1.5317169256021399</v>
+        <v>1.66250101299196</v>
       </c>
       <c r="J169" t="s">
         <v>21</v>
       </c>
       <c r="K169" t="s">
-        <v>208</v>
-      </c>
-      <c r="N169" t="s">
-        <v>206</v>
+        <v>214</v>
+      </c>
+      <c r="L169" t="s">
+        <v>215</v>
+      </c>
+      <c r="M169" t="s">
+        <v>216</v>
       </c>
       <c r="O169" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="170" spans="1:15">
       <c r="A170" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B170" s="1">
-        <v>40659.85193287037</v>
+        <v>42109.90828703704</v>
       </c>
       <c r="C170" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D170">
-        <v>2.46599999999999</v>
+        <v>20.206</v>
       </c>
       <c r="E170">
-        <v>0.154</v>
+        <v>1.0740000000000001</v>
       </c>
       <c r="F170">
-        <v>20.613000000000302</v>
+        <v>21.203000000000401</v>
       </c>
       <c r="G170">
         <v>1856</v>
       </c>
       <c r="H170">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I170">
-        <v>1.5324814378691001</v>
+        <v>1.63488299912919</v>
       </c>
       <c r="J170" t="s">
         <v>21</v>
       </c>
       <c r="K170" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="L170" t="s">
-        <v>210</v>
-      </c>
-      <c r="N170" t="s">
-        <v>206</v>
+        <v>218</v>
+      </c>
+      <c r="M170" t="s">
+        <v>216</v>
       </c>
       <c r="O170" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="171" spans="1:15">
       <c r="A171" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B171" s="1">
-        <v>40659.853425925925</v>
+        <v>42109.910219907404</v>
       </c>
       <c r="C171" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D171">
-        <v>5.2539999999999996</v>
+        <v>20.748999999999999</v>
       </c>
       <c r="E171">
-        <v>0.26300000000000001</v>
+        <v>1.0349999999999999</v>
       </c>
       <c r="F171">
-        <v>43.096000000000501</v>
+        <v>21.721999999999799</v>
       </c>
       <c r="G171">
-        <v>3713</v>
+        <v>1856</v>
       </c>
       <c r="H171">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I171">
-        <v>1.67947876411185</v>
+        <v>1</v>
       </c>
       <c r="J171" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K171" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="L171" t="s">
-        <v>210</v>
-      </c>
-      <c r="N171" t="s">
-        <v>206</v>
+        <v>218</v>
+      </c>
+      <c r="M171" t="s">
+        <v>216</v>
       </c>
       <c r="O171" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="172" spans="1:15">
       <c r="A172" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B172" s="1">
-        <v>40659.854687500003</v>
+        <v>42109.911585648151</v>
       </c>
       <c r="C172" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D172">
-        <v>5.2880000000000003</v>
+        <v>20.614000000000001</v>
       </c>
       <c r="E172">
-        <v>0.29799999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="F172">
-        <v>58.8149999999996</v>
+        <v>21.542999999999701</v>
       </c>
       <c r="G172">
-        <v>3713</v>
+        <v>1856</v>
       </c>
       <c r="H172">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I172">
-        <v>1.67947876411185</v>
+        <v>0.99</v>
       </c>
       <c r="J172" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K172" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="L172" t="s">
-        <v>212</v>
-      </c>
-      <c r="N172" t="s">
-        <v>206</v>
+        <v>218</v>
+      </c>
+      <c r="M172" t="s">
+        <v>216</v>
       </c>
       <c r="O172" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="173" spans="1:15">
       <c r="A173" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B173" s="1">
-        <v>40659.856979166667</v>
+        <v>42109.918564814812</v>
       </c>
       <c r="C173" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="D173">
-        <v>9.4990000000000094</v>
+        <v>20.510999999999999</v>
       </c>
       <c r="E173">
-        <v>0.66600000000000004</v>
+        <v>1.0049999999999999</v>
       </c>
       <c r="F173">
-        <v>45.574000000000503</v>
+        <v>21.440000000000499</v>
       </c>
       <c r="G173">
-        <v>3713</v>
+        <v>1856</v>
       </c>
       <c r="H173">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I173">
-        <v>1.6391630597812601</v>
+        <v>1.63488299912919</v>
       </c>
       <c r="J173" t="s">
         <v>21</v>
       </c>
       <c r="K173" t="s">
-        <v>213</v>
-      </c>
-      <c r="N173" t="s">
-        <v>206</v>
+        <v>217</v>
+      </c>
+      <c r="L173" t="s">
+        <v>218</v>
+      </c>
+      <c r="M173" t="s">
+        <v>216</v>
       </c>
       <c r="O173" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="174" spans="1:15">
       <c r="A174" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B174" s="1">
-        <v>40659.860312500001</v>
+        <v>42121.844583333332</v>
       </c>
       <c r="C174" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="D174">
-        <v>9.7119999999999909</v>
+        <v>3.0630000000000002</v>
       </c>
       <c r="E174">
-        <v>0.70799999999999996</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="F174">
-        <v>46.558</v>
+        <v>93.864000000000502</v>
       </c>
       <c r="G174">
-        <v>3713</v>
+        <v>1856</v>
       </c>
       <c r="H174">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I174">
-        <v>1.6391630597812601</v>
+        <v>1.6325571524315501</v>
       </c>
       <c r="J174" t="s">
         <v>21</v>
       </c>
       <c r="K174" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="N174" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="O174" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="175" spans="1:15">
       <c r="A175" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B175" s="1">
-        <v>40659.863749999997</v>
+        <v>42121.847118055557</v>
       </c>
       <c r="C175" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="D175">
-        <v>5.5699999999999896</v>
+        <v>2.976</v>
       </c>
       <c r="E175">
-        <v>0.30600000000000099</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="F175">
-        <v>60.558</v>
+        <v>100.997</v>
       </c>
       <c r="G175">
-        <v>3713</v>
+        <v>1856</v>
       </c>
       <c r="H175">
         <v>93</v>
       </c>
       <c r="I175">
-        <v>1.5823919857797799</v>
+        <v>1.5866800350352499</v>
       </c>
       <c r="J175" t="s">
         <v>21</v>
       </c>
       <c r="K175" t="s">
-        <v>215</v>
-      </c>
-      <c r="L175" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="N175" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="O175" t="s">
         <v>39</v>
@@ -8448,379 +8499,678 @@
     </row>
     <row r="176" spans="1:15">
       <c r="A176" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B176" s="1">
-        <v>40659.86519675926</v>
+        <v>42121.848344907405</v>
       </c>
       <c r="C176" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D176">
-        <v>4.8290000000000104</v>
+        <v>2.48</v>
       </c>
       <c r="E176">
-        <v>0.30399999999999799</v>
+        <v>0.13899999999999901</v>
       </c>
       <c r="F176">
-        <v>55.797999999999803</v>
+        <v>9.2620000000006293</v>
       </c>
       <c r="G176">
-        <v>3713</v>
+        <v>1856</v>
       </c>
       <c r="H176">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="I176">
-        <v>1.6568002530577599</v>
+        <v>1.5317169256021399</v>
       </c>
       <c r="J176" t="s">
         <v>21</v>
       </c>
       <c r="K176" t="s">
-        <v>216</v>
-      </c>
-      <c r="L176" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="N176" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="O176" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="177" spans="1:15">
       <c r="A177" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B177" s="1">
-        <v>40659.867673611108</v>
+        <v>42121.85193287037</v>
       </c>
       <c r="C177" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D177">
-        <v>4.9149999999999903</v>
+        <v>2.46599999999999</v>
       </c>
       <c r="E177">
-        <v>0.315999999999999</v>
+        <v>0.154</v>
       </c>
       <c r="F177">
-        <v>62.327999999999498</v>
+        <v>20.613000000000302</v>
       </c>
       <c r="G177">
-        <v>3713</v>
+        <v>1856</v>
       </c>
       <c r="H177">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="I177">
-        <v>1.65692310884533</v>
+        <v>1.5324814378691001</v>
       </c>
       <c r="J177" t="s">
         <v>21</v>
       </c>
       <c r="K177" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="L177" t="s">
-        <v>212</v>
-      </c>
-      <c r="M177" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="N177" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="O177" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="178" spans="1:15">
       <c r="A178" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B178" s="1">
-        <v>40659.869687500002</v>
+        <v>42121.853425925925</v>
       </c>
       <c r="C178" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D178">
-        <v>4.9019999999999904</v>
+        <v>5.2539999999999996</v>
       </c>
       <c r="E178">
-        <v>0.30499999999999999</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="F178">
-        <v>52.561000000000597</v>
+        <v>43.096000000000501</v>
       </c>
       <c r="G178">
         <v>3713</v>
       </c>
       <c r="H178">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="I178">
-        <v>1.65804340818409</v>
+        <v>1.67947876411185</v>
       </c>
       <c r="J178" t="s">
         <v>21</v>
       </c>
       <c r="K178" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="L178" t="s">
-        <v>218</v>
-      </c>
-      <c r="M178" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="N178" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="O178" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="179" spans="1:15">
       <c r="A179" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B179" s="1">
-        <v>40661.520416666666</v>
+        <v>42121.854687500003</v>
       </c>
       <c r="C179" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="D179">
-        <v>147.87</v>
+        <v>5.2880000000000003</v>
       </c>
       <c r="E179">
-        <v>0.47</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="F179">
-        <v>149.09</v>
+        <v>58.8149999999996</v>
       </c>
       <c r="G179">
-        <v>1861</v>
+        <v>3713</v>
       </c>
       <c r="H179">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I179">
-        <v>0.879687868181247</v>
+        <v>1.67947876411185</v>
       </c>
       <c r="J179" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K179" t="s">
-        <v>220</v>
+        <v>226</v>
+      </c>
+      <c r="L179" t="s">
+        <v>227</v>
       </c>
       <c r="N179" t="s">
         <v>221</v>
       </c>
       <c r="O179" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="180" spans="1:15">
       <c r="A180" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B180" s="1">
-        <v>40661.526898148149</v>
+        <v>42121.856979166667</v>
       </c>
       <c r="C180" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="D180">
-        <v>437.02</v>
+        <v>9.4990000000000094</v>
       </c>
       <c r="E180">
-        <v>2.4500000000000002</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="F180">
-        <v>440.29</v>
+        <v>45.574000000000503</v>
       </c>
       <c r="G180">
-        <v>3718</v>
+        <v>3713</v>
       </c>
       <c r="H180">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I180">
-        <v>0.816933944528761</v>
+        <v>1.6391630597812601</v>
       </c>
       <c r="J180" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K180" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="N180" t="s">
         <v>221</v>
       </c>
       <c r="O180" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="181" spans="1:15">
       <c r="A181" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B181" s="1">
-        <v>40661.551562499997</v>
+        <v>42121.860312500001</v>
       </c>
       <c r="C181" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="D181">
-        <v>1400.45</v>
+        <v>9.7119999999999909</v>
       </c>
       <c r="E181">
-        <v>11.27</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="F181">
-        <v>1413.65</v>
+        <v>46.558</v>
       </c>
       <c r="G181">
-        <v>7429</v>
+        <v>3713</v>
       </c>
       <c r="H181">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I181">
-        <v>0.75435019649979396</v>
+        <v>1.6391630597812601</v>
       </c>
       <c r="J181" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K181" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N181" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="O181" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="182" spans="1:15">
       <c r="A182" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B182" s="1">
-        <v>40661.621365740742</v>
+        <v>42121.863749999997</v>
       </c>
       <c r="C182" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="D182">
-        <v>3097.3</v>
+        <v>5.5699999999999896</v>
       </c>
       <c r="E182">
-        <v>23.74</v>
+        <v>0.30600000000000099</v>
       </c>
       <c r="F182">
-        <v>3132.3</v>
+        <v>60.558</v>
       </c>
       <c r="G182">
-        <v>11144</v>
+        <v>3713</v>
       </c>
       <c r="H182">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I182">
-        <v>0.72482857368610298</v>
+        <v>1.5823919857797799</v>
       </c>
       <c r="J182" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K182" t="s">
-        <v>224</v>
+        <v>230</v>
+      </c>
+      <c r="L182" t="s">
+        <v>227</v>
       </c>
       <c r="N182" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="O182" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="183" spans="1:15">
       <c r="A183" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="B183" s="1">
-        <v>40652.307604166665</v>
+        <v>42121.86519675926</v>
       </c>
       <c r="C183" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="D183">
-        <v>4.0419999999999998</v>
+        <v>4.8290000000000104</v>
       </c>
       <c r="E183">
-        <v>0.107</v>
+        <v>0.30399999999999799</v>
       </c>
       <c r="F183">
-        <v>12.631999999999801</v>
+        <v>55.797999999999803</v>
       </c>
       <c r="G183">
-        <v>1856</v>
+        <v>3713</v>
       </c>
       <c r="H183">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I183">
-        <v>1.5610810802361099</v>
+        <v>1.6568002530577599</v>
       </c>
       <c r="J183" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K183" t="s">
+        <v>231</v>
+      </c>
+      <c r="L183" t="s">
         <v>227</v>
       </c>
+      <c r="N183" t="s">
+        <v>229</v>
+      </c>
       <c r="O183" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="184" spans="1:15">
       <c r="A184" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="B184" s="1">
-        <v>40652.309560185182</v>
+        <v>42121.867673611108</v>
       </c>
       <c r="C184" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="D184">
-        <v>7.5640000000000001</v>
+        <v>4.9149999999999903</v>
       </c>
       <c r="E184">
-        <v>0.217</v>
+        <v>0.315999999999999</v>
       </c>
       <c r="F184">
-        <v>21.059999999999899</v>
+        <v>62.327999999999498</v>
       </c>
       <c r="G184">
         <v>3713</v>
       </c>
       <c r="H184">
+        <v>80</v>
+      </c>
+      <c r="I184">
+        <v>1.65692310884533</v>
+      </c>
+      <c r="J184" t="s">
+        <v>21</v>
+      </c>
+      <c r="K184" t="s">
+        <v>231</v>
+      </c>
+      <c r="L184" t="s">
+        <v>227</v>
+      </c>
+      <c r="M184" t="s">
+        <v>232</v>
+      </c>
+      <c r="N184" t="s">
+        <v>229</v>
+      </c>
+      <c r="O184" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15">
+      <c r="A185" t="s">
+        <v>208</v>
+      </c>
+      <c r="B185" s="1">
+        <v>42121.869687500002</v>
+      </c>
+      <c r="C185" t="s">
+        <v>211</v>
+      </c>
+      <c r="D185">
+        <v>4.9019999999999904</v>
+      </c>
+      <c r="E185">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="F185">
+        <v>52.561000000000597</v>
+      </c>
+      <c r="G185">
+        <v>3713</v>
+      </c>
+      <c r="H185">
+        <v>80</v>
+      </c>
+      <c r="I185">
+        <v>1.65804340818409</v>
+      </c>
+      <c r="J185" t="s">
+        <v>21</v>
+      </c>
+      <c r="K185" t="s">
+        <v>217</v>
+      </c>
+      <c r="L185" t="s">
+        <v>233</v>
+      </c>
+      <c r="M185" t="s">
+        <v>232</v>
+      </c>
+      <c r="N185" t="s">
+        <v>229</v>
+      </c>
+      <c r="O185" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15">
+      <c r="A186" t="s">
+        <v>234</v>
+      </c>
+      <c r="B186" s="1">
+        <v>42123.520416666666</v>
+      </c>
+      <c r="C186" t="s">
+        <v>209</v>
+      </c>
+      <c r="D186">
+        <v>147.87</v>
+      </c>
+      <c r="E186">
+        <v>0.47</v>
+      </c>
+      <c r="F186">
+        <v>149.09</v>
+      </c>
+      <c r="G186">
+        <v>1861</v>
+      </c>
+      <c r="H186">
+        <v>94</v>
+      </c>
+      <c r="I186">
+        <v>0.879687868181247</v>
+      </c>
+      <c r="J186" t="s">
+        <v>17</v>
+      </c>
+      <c r="K186" t="s">
+        <v>235</v>
+      </c>
+      <c r="N186" t="s">
+        <v>236</v>
+      </c>
+      <c r="O186" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15">
+      <c r="A187" t="s">
+        <v>234</v>
+      </c>
+      <c r="B187" s="1">
+        <v>42123.526898148149</v>
+      </c>
+      <c r="C187" t="s">
+        <v>209</v>
+      </c>
+      <c r="D187">
+        <v>437.02</v>
+      </c>
+      <c r="E187">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="F187">
+        <v>440.29</v>
+      </c>
+      <c r="G187">
+        <v>3718</v>
+      </c>
+      <c r="H187">
+        <v>94</v>
+      </c>
+      <c r="I187">
+        <v>0.816933944528761</v>
+      </c>
+      <c r="J187" t="s">
+        <v>17</v>
+      </c>
+      <c r="K187" t="s">
+        <v>237</v>
+      </c>
+      <c r="N187" t="s">
+        <v>236</v>
+      </c>
+      <c r="O187" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15">
+      <c r="A188" t="s">
+        <v>234</v>
+      </c>
+      <c r="B188" s="1">
+        <v>42123.551562499997</v>
+      </c>
+      <c r="C188" t="s">
+        <v>209</v>
+      </c>
+      <c r="D188">
+        <v>1400.45</v>
+      </c>
+      <c r="E188">
+        <v>11.27</v>
+      </c>
+      <c r="F188">
+        <v>1413.65</v>
+      </c>
+      <c r="G188">
+        <v>7429</v>
+      </c>
+      <c r="H188">
+        <v>94</v>
+      </c>
+      <c r="I188">
+        <v>0.75435019649979396</v>
+      </c>
+      <c r="J188" t="s">
+        <v>17</v>
+      </c>
+      <c r="K188" t="s">
+        <v>238</v>
+      </c>
+      <c r="N188" t="s">
+        <v>236</v>
+      </c>
+      <c r="O188" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15">
+      <c r="A189" t="s">
+        <v>234</v>
+      </c>
+      <c r="B189" s="1">
+        <v>42123.621365740742</v>
+      </c>
+      <c r="C189" t="s">
+        <v>209</v>
+      </c>
+      <c r="D189">
+        <v>3097.3</v>
+      </c>
+      <c r="E189">
+        <v>23.74</v>
+      </c>
+      <c r="F189">
+        <v>3132.3</v>
+      </c>
+      <c r="G189">
+        <v>11144</v>
+      </c>
+      <c r="H189">
+        <v>94</v>
+      </c>
+      <c r="I189">
+        <v>0.72482857368610298</v>
+      </c>
+      <c r="J189" t="s">
+        <v>17</v>
+      </c>
+      <c r="K189" t="s">
+        <v>239</v>
+      </c>
+      <c r="N189" t="s">
+        <v>236</v>
+      </c>
+      <c r="O189" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15">
+      <c r="A190" t="s">
+        <v>240</v>
+      </c>
+      <c r="B190" s="1">
+        <v>42114.307604166665</v>
+      </c>
+      <c r="C190" t="s">
+        <v>241</v>
+      </c>
+      <c r="D190">
+        <v>4.0419999999999998</v>
+      </c>
+      <c r="E190">
+        <v>0.107</v>
+      </c>
+      <c r="F190">
+        <v>12.631999999999801</v>
+      </c>
+      <c r="G190">
+        <v>1856</v>
+      </c>
+      <c r="H190">
         <v>93</v>
       </c>
-      <c r="I184">
+      <c r="I190">
+        <v>1.5610810802361099</v>
+      </c>
+      <c r="J190" t="s">
+        <v>17</v>
+      </c>
+      <c r="K190" t="s">
+        <v>242</v>
+      </c>
+      <c r="O190" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15">
+      <c r="A191" t="s">
+        <v>240</v>
+      </c>
+      <c r="B191" s="1">
+        <v>42114.309560185182</v>
+      </c>
+      <c r="C191" t="s">
+        <v>241</v>
+      </c>
+      <c r="D191">
+        <v>7.5640000000000001</v>
+      </c>
+      <c r="E191">
+        <v>0.217</v>
+      </c>
+      <c r="F191">
+        <v>21.059999999999899</v>
+      </c>
+      <c r="G191">
+        <v>3713</v>
+      </c>
+      <c r="H191">
+        <v>93</v>
+      </c>
+      <c r="I191">
         <v>1.47755844028469</v>
       </c>
-      <c r="J184" t="s">
+      <c r="J191" t="s">
         <v>17</v>
       </c>
-      <c r="K184" t="s">
-        <v>227</v>
-      </c>
-      <c r="O184" t="s">
+      <c r="K191" t="s">
+        <v>242</v>
+      </c>
+      <c r="O191" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>